<commit_message>
adding in decision tree modeling
</commit_message>
<xml_diff>
--- a/Covertype_Prediction/Scripts/accuracy.xlsx
+++ b/Covertype_Prediction/Scripts/accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelateng/Documents/GitHub/Projects/Covertype_Prediction/Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6431CEFA-36FB-E742-9830-772DE9830A3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD999006-1DA7-F144-9282-FBD888F85EE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="440" windowWidth="16080" windowHeight="19700" xr2:uid="{281056B7-1BF2-7741-906E-052FB1D655A7}"/>
+    <workbookView xWindow="2860" yWindow="440" windowWidth="17320" windowHeight="17940" xr2:uid="{281056B7-1BF2-7741-906E-052FB1D655A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -64,14 +64,28 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Ensemble Voting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrained Models Based on Hyperparamter Search V2 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,11 +130,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -128,6 +153,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,20 +470,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87564167-29EF-F84B-B189-576ECAC9FD9C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +494,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -477,7 +509,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -488,7 +520,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -499,7 +531,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -510,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,7 +553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -531,6 +563,15 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.81</v>
+      </c>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{61C022B8-ABFA-D649-9902-A40E353C6A63}">

</xml_diff>

<commit_message>
added grid search for random forest
</commit_message>
<xml_diff>
--- a/Covertype_Prediction/Scripts/accuracy.xlsx
+++ b/Covertype_Prediction/Scripts/accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelateng/Documents/GitHub/Projects/Covertype_Prediction/Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD999006-1DA7-F144-9282-FBD888F85EE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6DD646-9787-5447-A476-41BD0476901B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="440" windowWidth="17320" windowHeight="17940" xr2:uid="{281056B7-1BF2-7741-906E-052FB1D655A7}"/>
+    <workbookView xWindow="14300" yWindow="440" windowWidth="19580" windowHeight="19700" xr2:uid="{281056B7-1BF2-7741-906E-052FB1D655A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,22 +130,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -153,7 +142,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -473,7 +461,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +482,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -508,6 +496,9 @@
       <c r="C2" s="4">
         <v>0.82</v>
       </c>
+      <c r="D2" s="4">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -519,6 +510,7 @@
       <c r="C3" s="4">
         <v>0.8</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -530,6 +522,7 @@
       <c r="C4" s="4">
         <v>0.73</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -541,6 +534,9 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="4">
+        <v>0.51</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -552,6 +548,7 @@
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -563,15 +560,17 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.81</v>
       </c>
       <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{61C022B8-ABFA-D649-9902-A40E353C6A63}">

</xml_diff>